<commit_message>
feat: formula and table functions [sort, filter]
</commit_message>
<xml_diff>
--- a/public/assets/testing/(shortened) (csv) SHA Ratesheet eff 20241029 - APAC.xlsx
+++ b/public/assets/testing/(shortened) (csv) SHA Ratesheet eff 20241029 - APAC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CGOMAL\OneDrive - Cathay Pacific Airways Limited\Desktop\Project\rate-sheet-generator\cathay-cargo-harpy\public\assets\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B157B39E-1142-4B7C-A83C-1EC1FDDF2AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BAD6A4-878D-4DC6-90AB-B5B3B6B10839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Standard Rate (RM)" sheetId="16" r:id="rId1"/>
@@ -8706,7 +8706,7 @@
   <dimension ref="A1:AL32"/>
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15318,6 +15318,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="c5381946-f1d1-449f-b695-d98d204cc1c9">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="c5381946-f1d1-449f-b695-d98d204cc1c9" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="75c5e37f-bc1e-40b7-ac00-1ab7acfb489c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009D8784BC270A2B458FD6DC47BBDD8083" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d0b5628bed754749cf53d2271575fbf9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="75c5e37f-bc1e-40b7-ac00-1ab7acfb489c" xmlns:ns3="c5381946-f1d1-449f-b695-d98d204cc1c9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7fae9e5550cb33a7bb119824a5700ac8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -15583,26 +15603,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="c5381946-f1d1-449f-b695-d98d204cc1c9">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="c5381946-f1d1-449f-b695-d98d204cc1c9" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="75c5e37f-bc1e-40b7-ac00-1ab7acfb489c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -15613,6 +15613,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{990DCB4B-FBBF-4997-8C1B-1027DBEC0554}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c5381946-f1d1-449f-b695-d98d204cc1c9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="75c5e37f-bc1e-40b7-ac00-1ab7acfb489c"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30BDA860-E7BE-4FA0-B022-CDB54E247940}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15632,18 +15644,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{990DCB4B-FBBF-4997-8C1B-1027DBEC0554}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c5381946-f1d1-449f-b695-d98d204cc1c9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="75c5e37f-bc1e-40b7-ac00-1ab7acfb489c"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47809CAB-73CD-4E13-B718-ADA289F0A22D}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
some styling of code
</commit_message>
<xml_diff>
--- a/public/assets/testing/(shortened) (csv) SHA Ratesheet eff 20241029 - APAC.xlsx
+++ b/public/assets/testing/(shortened) (csv) SHA Ratesheet eff 20241029 - APAC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CGOMAL\OneDrive - Cathay Pacific Airways Limited\Desktop\Project\rate-sheet-generator\cathay-cargo-harpy\public\assets\testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\csluk2001\cathay-cargo\rate-sheet\cathay-cargo-harpy\public\assets\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BAD6A4-878D-4DC6-90AB-B5B3B6B10839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2575B448-0FE6-4C93-8F01-8845BCC6B10E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1515" uniqueCount="989">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1728" uniqueCount="1051">
   <si>
     <t>NET</t>
   </si>
@@ -3010,6 +3010,253 @@
   </si>
   <si>
     <t>Perishables</t>
+  </si>
+  <si>
+    <t>SHA</t>
+  </si>
+  <si>
+    <t>J33+5</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J34+5</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J35+5</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J33+2</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J34+2</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J35+2</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J33+1</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J34+1</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J35+1</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J39+5</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J40+5</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J41+5</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J42+5</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J43+5</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J44+5</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J45+5</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J46+5</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J47+5</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J48+5</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J49+5</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J50+5</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J51+5</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J51+2</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J50+2</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J49+2</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J48+2</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J47+2</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J46+2</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J45+2</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J44+2</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J43+2</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J42+2</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J41+2</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J40+2</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J39+2</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J39+1</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J40+1</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J41+1</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J42+1</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J43+1</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J44+1</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J45+1</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J46+1</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J47+1</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J48+1</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J49+1</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J50+1</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>J51+1</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>L22-1</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>L21-1</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>L20-1</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>L19-1</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>L18-1</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>L17-1</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>L16-1</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>L15-1</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>L14-1</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>L13-1</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>L12-1</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>L11-1</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>L10-1</t>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3017,18 +3264,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
-    <numFmt numFmtId="164" formatCode="[$USD]\ #,##0.0"/>
-    <numFmt numFmtId="165" formatCode="[$-409]d/mmm/yy;@"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="[$-409]d\-mmm;@"/>
-    <numFmt numFmtId="168" formatCode="#,##0.0"/>
-    <numFmt numFmtId="169" formatCode="\+0.00"/>
+    <numFmt numFmtId="176" formatCode="[$USD]\ #,##0.0"/>
+    <numFmt numFmtId="177" formatCode="[$-409]d/mmm/yy;@"/>
+    <numFmt numFmtId="178" formatCode="0.0"/>
+    <numFmt numFmtId="179" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="180" formatCode="#,##0.0"/>
+    <numFmt numFmtId="181" formatCode="\+0.00"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3068,13 +3315,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -3087,7 +3334,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -3323,22 +3570,22 @@
   </borders>
   <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3359,7 +3606,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="5">
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" xfId="5">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -3368,10 +3615,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="5" borderId="3" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="5" borderId="3" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="5" borderId="4" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="5" borderId="4" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -3392,7 +3639,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="5" borderId="4" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="5" borderId="4" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="5" applyNumberFormat="1" applyBorder="1">
@@ -3434,7 +3681,7 @@
     <xf numFmtId="2" fontId="5" fillId="5" borderId="4" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="5" borderId="1" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="5" borderId="1" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -3494,56 +3741,56 @@
     <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="5" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="5" fillId="0" borderId="5" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="12" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="5" fillId="0" borderId="12" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="9" fillId="0" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="7" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="7" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="7" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="7" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="7" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="7" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="9" fillId="7" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="5" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3561,100 +3808,100 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="11" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="11" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="12" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="12" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="11" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="11" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="12" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="12" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="10" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="10" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="9" fillId="0" borderId="10" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="3" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="2" borderId="3" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="3" borderId="14" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="3" borderId="14" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="3" borderId="15" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="3" borderId="15" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="3" borderId="13" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="3" borderId="13" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="4" borderId="2" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="4" borderId="2" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="4" borderId="3" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="4" borderId="3" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="4" borderId="4" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="4" borderId="4" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="3" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="2" borderId="3" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="5" borderId="2" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="5" borderId="2" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="6" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="6" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="9" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="9" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="6" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="6" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="9" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="9" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="8" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="8" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="5" fillId="0" borderId="8" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="11" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="11" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="5" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="5" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="12" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="12" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="11" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="11" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="5" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="5" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="12" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="12" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="10" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="10" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="5" fillId="0" borderId="10" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -3666,25 +3913,25 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="14" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="14" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="15" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="15" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="13" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="13" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="14" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="14" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="15" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="15" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="13" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="13" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="9" fillId="0" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3696,25 +3943,25 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="13" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="7" borderId="14" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="7" borderId="14" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="7" borderId="15" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="7" borderId="15" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="7" borderId="13" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="7" borderId="13" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="7" borderId="14" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="7" borderId="14" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="7" borderId="15" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="7" borderId="15" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="7" borderId="13" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="7" borderId="13" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="7" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="7" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="9" fillId="7" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3723,16 +3970,16 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="7" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="7" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="7" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="7" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="7" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="7" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="7" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="7" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="10" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3741,70 +3988,70 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="12" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="7" borderId="11" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="7" borderId="11" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="7" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="7" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="7" borderId="12" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="7" borderId="12" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="7" borderId="11" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="7" borderId="11" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="7" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="7" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="7" borderId="12" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="7" borderId="12" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="7" borderId="10" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="7" borderId="10" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="9" fillId="7" borderId="10" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="6" borderId="4" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="5" fillId="6" borderId="4" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="5" borderId="2" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="5" borderId="2" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="5" borderId="1" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="5" borderId="1" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="3" borderId="4" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="3" borderId="4" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="4" borderId="1" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="4" borderId="1" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="8" borderId="2" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="8" borderId="2" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="8" borderId="3" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="8" borderId="3" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="8" borderId="4" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="8" borderId="4" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="8" borderId="4" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="8" borderId="4" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="8" borderId="2" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="8" borderId="2" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="8" borderId="1" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="8" borderId="1" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="6" borderId="4" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="5" fillId="6" borderId="4" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="4" borderId="1" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="1" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="1" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="1" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="5" borderId="1" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3813,10 +4060,49 @@
     <xf numFmtId="2" fontId="5" fillId="5" borderId="2" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="5" borderId="2" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="5" borderId="2" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="6" borderId="4" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="5" fillId="6" borderId="4" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="2" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="3" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="4" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="14" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="15" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="13" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="7" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="7" borderId="6" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="7" borderId="0" xfId="5" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="7" borderId="9" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="7" borderId="8" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4110,18 +4396,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E45B05CD-A8F6-4940-B735-4143CE1CE717}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AL32"/>
+  <dimension ref="A1:AL51"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:AL51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="38" max="38" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="99.75">
+    <row r="1" spans="1:38" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -4231,7 +4517,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:38">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>13</v>
       </c>
@@ -4347,7 +4633,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="3" spans="1:38">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="109" t="s">
         <v>21</v>
       </c>
@@ -4491,7 +4777,7 @@
         <v>45594</v>
       </c>
     </row>
-    <row r="4" spans="1:38">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="109" t="s">
         <v>21</v>
       </c>
@@ -4636,7 +4922,7 @@
         <v>45594</v>
       </c>
     </row>
-    <row r="5" spans="1:38">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="72" t="s">
         <v>21</v>
       </c>
@@ -4781,7 +5067,7 @@
         <v>45594</v>
       </c>
     </row>
-    <row r="6" spans="1:38">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="72" t="s">
         <v>21</v>
       </c>
@@ -4926,7 +5212,7 @@
         <v>45594</v>
       </c>
     </row>
-    <row r="7" spans="1:38">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="72" t="s">
         <v>21</v>
       </c>
@@ -5071,7 +5357,7 @@
         <v>45594</v>
       </c>
     </row>
-    <row r="8" spans="1:38">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" s="72" t="s">
         <v>21</v>
       </c>
@@ -5216,7 +5502,7 @@
         <v>45594</v>
       </c>
     </row>
-    <row r="9" spans="1:38">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" s="72" t="s">
         <v>21</v>
       </c>
@@ -5361,7 +5647,7 @@
         <v>45594</v>
       </c>
     </row>
-    <row r="10" spans="1:38">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="72" t="s">
         <v>21</v>
       </c>
@@ -5506,7 +5792,7 @@
         <v>45594</v>
       </c>
     </row>
-    <row r="11" spans="1:38">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" s="72" t="s">
         <v>21</v>
       </c>
@@ -5651,7 +5937,7 @@
         <v>45594</v>
       </c>
     </row>
-    <row r="12" spans="1:38">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" s="74" t="s">
         <v>21</v>
       </c>
@@ -5796,7 +6082,7 @@
         <v>45594</v>
       </c>
     </row>
-    <row r="13" spans="1:38">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>21</v>
       </c>
@@ -5941,7 +6227,7 @@
         <v>45587</v>
       </c>
     </row>
-    <row r="14" spans="1:38">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>21</v>
       </c>
@@ -6089,7 +6375,7 @@
         <v>45587</v>
       </c>
     </row>
-    <row r="15" spans="1:38">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>21</v>
       </c>
@@ -6233,7 +6519,7 @@
         <v>45566</v>
       </c>
     </row>
-    <row r="16" spans="1:38">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>21</v>
       </c>
@@ -6378,7 +6664,7 @@
         <v>45587</v>
       </c>
     </row>
-    <row r="17" spans="1:38">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>21</v>
       </c>
@@ -6526,7 +6812,7 @@
         <v>45566</v>
       </c>
     </row>
-    <row r="18" spans="1:38">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>21</v>
       </c>
@@ -6671,7 +6957,7 @@
         <v>45587</v>
       </c>
     </row>
-    <row r="19" spans="1:38">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>21</v>
       </c>
@@ -6816,7 +7102,7 @@
         <v>45566</v>
       </c>
     </row>
-    <row r="20" spans="1:38">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>21</v>
       </c>
@@ -6961,7 +7247,7 @@
         <v>45587</v>
       </c>
     </row>
-    <row r="21" spans="1:38">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>21</v>
       </c>
@@ -7106,7 +7392,7 @@
         <v>45566</v>
       </c>
     </row>
-    <row r="22" spans="1:38">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>21</v>
       </c>
@@ -7251,7 +7537,7 @@
         <v>45587</v>
       </c>
     </row>
-    <row r="23" spans="1:38">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>21</v>
       </c>
@@ -7396,7 +7682,7 @@
         <v>45587</v>
       </c>
     </row>
-    <row r="24" spans="1:38">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>21</v>
       </c>
@@ -7540,7 +7826,7 @@
         <v>45587</v>
       </c>
     </row>
-    <row r="25" spans="1:38">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
         <v>21</v>
       </c>
@@ -7685,7 +7971,7 @@
         <v>45587</v>
       </c>
     </row>
-    <row r="26" spans="1:38">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
         <v>21</v>
       </c>
@@ -7830,7 +8116,7 @@
         <v>45566</v>
       </c>
     </row>
-    <row r="27" spans="1:38">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A27" s="119" t="s">
         <v>21</v>
       </c>
@@ -7974,7 +8260,7 @@
         <v>45594</v>
       </c>
     </row>
-    <row r="28" spans="1:38">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A28" s="71" t="s">
         <v>21</v>
       </c>
@@ -8118,7 +8404,7 @@
         <v>45594</v>
       </c>
     </row>
-    <row r="29" spans="1:38">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A29" s="71" t="s">
         <v>21</v>
       </c>
@@ -8262,7 +8548,7 @@
         <v>45594</v>
       </c>
     </row>
-    <row r="30" spans="1:38">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A30" s="71" t="s">
         <v>21</v>
       </c>
@@ -8406,7 +8692,7 @@
         <v>45594</v>
       </c>
     </row>
-    <row r="31" spans="1:38">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A31" s="72" t="s">
         <v>21</v>
       </c>
@@ -8550,7 +8836,7 @@
         <v>45594</v>
       </c>
     </row>
-    <row r="32" spans="1:38">
+    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A32" s="134" t="s">
         <v>21</v>
       </c>
@@ -8692,6 +8978,618 @@
       </c>
       <c r="AL32" s="143">
         <v>45594</v>
+      </c>
+    </row>
+    <row r="33" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>989</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33" s="162">
+        <f>H33+5</f>
+        <v>7.6</v>
+      </c>
+      <c r="F33" s="163">
+        <f>H33+2</f>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G33" s="163">
+        <f>H33+1</f>
+        <v>3.6</v>
+      </c>
+      <c r="H33" s="164">
+        <v>2.6</v>
+      </c>
+      <c r="AL33" s="165">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="34" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>989</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E34" s="166">
+        <f>H34+5</f>
+        <v>8.6</v>
+      </c>
+      <c r="F34" s="167">
+        <f>H34+2</f>
+        <v>5.6</v>
+      </c>
+      <c r="G34" s="167">
+        <f t="shared" ref="G34" si="40">H34+1</f>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="H34" s="168">
+        <v>3.6</v>
+      </c>
+      <c r="AL34" s="169">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="35" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A35" s="15" t="s">
+        <v>989</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E35" s="93">
+        <f t="shared" ref="E35" si="41">H35+5</f>
+        <v>8.6</v>
+      </c>
+      <c r="F35" s="94">
+        <f t="shared" ref="F35" si="42">H35+2</f>
+        <v>5.6</v>
+      </c>
+      <c r="G35" s="94">
+        <f>H35+1</f>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="H35" s="95">
+        <v>3.6</v>
+      </c>
+      <c r="AL35" s="100">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="36" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A36" s="15" t="s">
+        <v>989</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E36" s="93">
+        <v>2.6</v>
+      </c>
+      <c r="F36" s="94">
+        <v>2.6</v>
+      </c>
+      <c r="G36" s="94">
+        <v>2.6</v>
+      </c>
+      <c r="H36" s="95">
+        <v>2.6</v>
+      </c>
+      <c r="AL36" s="100">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="37" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A37" s="15" t="s">
+        <v>989</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E37" s="93">
+        <v>2.6</v>
+      </c>
+      <c r="F37" s="94">
+        <v>2.6</v>
+      </c>
+      <c r="G37" s="94">
+        <v>2.6</v>
+      </c>
+      <c r="H37" s="95">
+        <v>2.6</v>
+      </c>
+      <c r="AL37" s="100">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="38" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A38" s="17" t="s">
+        <v>989</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E38" s="101">
+        <v>2.6</v>
+      </c>
+      <c r="F38" s="102">
+        <v>2.6</v>
+      </c>
+      <c r="G38" s="102">
+        <v>2.6</v>
+      </c>
+      <c r="H38" s="103">
+        <v>2.6</v>
+      </c>
+      <c r="AL38" s="108">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="39" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A39" s="15" t="s">
+        <v>989</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E39" s="93">
+        <f>H39+5</f>
+        <v>15.2</v>
+      </c>
+      <c r="F39" s="94">
+        <f t="shared" ref="F39:F40" si="43">H39+2</f>
+        <v>12.2</v>
+      </c>
+      <c r="G39" s="94">
+        <f t="shared" ref="G39:G40" si="44">H39+1</f>
+        <v>11.2</v>
+      </c>
+      <c r="H39" s="95">
+        <f>J10-1</f>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="AL39" s="100">
+        <v>45587</v>
+      </c>
+    </row>
+    <row r="40" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A40" s="15" t="s">
+        <v>989</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E40" s="93">
+        <f t="shared" ref="E40" si="45">H40+5</f>
+        <v>15.2</v>
+      </c>
+      <c r="F40" s="94">
+        <f t="shared" si="43"/>
+        <v>12.2</v>
+      </c>
+      <c r="G40" s="94">
+        <f t="shared" si="44"/>
+        <v>11.2</v>
+      </c>
+      <c r="H40" s="95">
+        <f>J11-1</f>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="AL40" s="100">
+        <v>45587</v>
+      </c>
+    </row>
+    <row r="41" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A41" s="15" t="s">
+        <v>989</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E41" s="93">
+        <f>H41+5</f>
+        <v>15.2</v>
+      </c>
+      <c r="F41" s="94">
+        <f>H41+2</f>
+        <v>12.2</v>
+      </c>
+      <c r="G41" s="94">
+        <f>H41+1</f>
+        <v>11.2</v>
+      </c>
+      <c r="H41" s="95">
+        <f>J12-1</f>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="AL41" s="100">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="42" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A42" s="15" t="s">
+        <v>989</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E42" s="93">
+        <f t="shared" ref="E42:E45" si="46">H42+5</f>
+        <v>18.5</v>
+      </c>
+      <c r="F42" s="94">
+        <f t="shared" ref="F42:F45" si="47">H42+2</f>
+        <v>15.5</v>
+      </c>
+      <c r="G42" s="94">
+        <f t="shared" ref="G42:G45" si="48">H42+1</f>
+        <v>14.5</v>
+      </c>
+      <c r="H42" s="95">
+        <f>J13-1</f>
+        <v>13.5</v>
+      </c>
+      <c r="AL42" s="100">
+        <v>45587</v>
+      </c>
+    </row>
+    <row r="43" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A43" s="15" t="s">
+        <v>989</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D43" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E43" s="93">
+        <f t="shared" si="46"/>
+        <v>16.2</v>
+      </c>
+      <c r="F43" s="94">
+        <f t="shared" si="47"/>
+        <v>13.2</v>
+      </c>
+      <c r="G43" s="94">
+        <f t="shared" si="48"/>
+        <v>12.2</v>
+      </c>
+      <c r="H43" s="95">
+        <f>J14-1</f>
+        <v>11.2</v>
+      </c>
+      <c r="AL43" s="100">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="44" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A44" s="15" t="s">
+        <v>989</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D44" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E44" s="93">
+        <f t="shared" si="46"/>
+        <v>18.5</v>
+      </c>
+      <c r="F44" s="94">
+        <f t="shared" si="47"/>
+        <v>15.5</v>
+      </c>
+      <c r="G44" s="94">
+        <f t="shared" si="48"/>
+        <v>14.5</v>
+      </c>
+      <c r="H44" s="95">
+        <f>J15-1</f>
+        <v>13.5</v>
+      </c>
+      <c r="AL44" s="100">
+        <v>45587</v>
+      </c>
+    </row>
+    <row r="45" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A45" s="15" t="s">
+        <v>989</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D45" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E45" s="93">
+        <f t="shared" si="46"/>
+        <v>16.2</v>
+      </c>
+      <c r="F45" s="94">
+        <f t="shared" si="47"/>
+        <v>13.2</v>
+      </c>
+      <c r="G45" s="94">
+        <f t="shared" si="48"/>
+        <v>12.2</v>
+      </c>
+      <c r="H45" s="95">
+        <f>J16-1</f>
+        <v>11.2</v>
+      </c>
+      <c r="AL45" s="100">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="46" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A46" s="170" t="s">
+        <v>989</v>
+      </c>
+      <c r="B46" s="170" t="s">
+        <v>37</v>
+      </c>
+      <c r="C46" s="170" t="s">
+        <v>38</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E46" s="171">
+        <f>H46+5</f>
+        <v>12.7</v>
+      </c>
+      <c r="F46" s="172">
+        <f>H46+2</f>
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="G46" s="172">
+        <f>H46+1</f>
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="H46" s="173">
+        <f>J17-1</f>
+        <v>7.6999999999999993</v>
+      </c>
+      <c r="AL46" s="174">
+        <v>45587</v>
+      </c>
+    </row>
+    <row r="47" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A47" s="15" t="s">
+        <v>989</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D47" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E47" s="93">
+        <f t="shared" ref="E47:E49" si="49">H47+5</f>
+        <v>16.2</v>
+      </c>
+      <c r="F47" s="94">
+        <f t="shared" ref="F47:F49" si="50">H47+2</f>
+        <v>13.2</v>
+      </c>
+      <c r="G47" s="94">
+        <f t="shared" ref="G47:G49" si="51">H47+1</f>
+        <v>12.2</v>
+      </c>
+      <c r="H47" s="95">
+        <f>J18-1</f>
+        <v>11.2</v>
+      </c>
+      <c r="AL47" s="100">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="48" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A48" s="15" t="s">
+        <v>989</v>
+      </c>
+      <c r="B48" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E48" s="93">
+        <f t="shared" si="49"/>
+        <v>15</v>
+      </c>
+      <c r="F48" s="94">
+        <f t="shared" si="50"/>
+        <v>12</v>
+      </c>
+      <c r="G48" s="94">
+        <f t="shared" si="51"/>
+        <v>11</v>
+      </c>
+      <c r="H48" s="95">
+        <f>J19-1</f>
+        <v>10</v>
+      </c>
+      <c r="AL48" s="100">
+        <v>45587</v>
+      </c>
+    </row>
+    <row r="49" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A49" s="15" t="s">
+        <v>989</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D49" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E49" s="93">
+        <f t="shared" si="49"/>
+        <v>16.2</v>
+      </c>
+      <c r="F49" s="94">
+        <f t="shared" si="50"/>
+        <v>13.2</v>
+      </c>
+      <c r="G49" s="94">
+        <f t="shared" si="51"/>
+        <v>12.2</v>
+      </c>
+      <c r="H49" s="95">
+        <f>J20-1</f>
+        <v>11.2</v>
+      </c>
+      <c r="AL49" s="100">
+        <v>45587</v>
+      </c>
+    </row>
+    <row r="50" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A50" s="170" t="s">
+        <v>989</v>
+      </c>
+      <c r="B50" s="170" t="s">
+        <v>37</v>
+      </c>
+      <c r="C50" s="170" t="s">
+        <v>42</v>
+      </c>
+      <c r="D50" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E50" s="171">
+        <f>H50+5</f>
+        <v>18.5</v>
+      </c>
+      <c r="F50" s="172">
+        <f>H50+2</f>
+        <v>15.5</v>
+      </c>
+      <c r="G50" s="172">
+        <f>H50+1</f>
+        <v>14.5</v>
+      </c>
+      <c r="H50" s="173">
+        <f>J21-1</f>
+        <v>13.5</v>
+      </c>
+      <c r="AL50" s="174">
+        <v>45587</v>
+      </c>
+    </row>
+    <row r="51" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A51" s="17" t="s">
+        <v>989</v>
+      </c>
+      <c r="B51" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D51" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E51" s="101">
+        <f t="shared" ref="E51" si="52">H51+5</f>
+        <v>16.2</v>
+      </c>
+      <c r="F51" s="102">
+        <f t="shared" ref="F51" si="53">H51+2</f>
+        <v>13.2</v>
+      </c>
+      <c r="G51" s="102">
+        <f t="shared" ref="G51" si="54">H51+1</f>
+        <v>12.2</v>
+      </c>
+      <c r="H51" s="103">
+        <f>J22-1</f>
+        <v>11.2</v>
+      </c>
+      <c r="AL51" s="108">
+        <v>45587</v>
       </c>
     </row>
   </sheetData>
@@ -8703,18 +9601,18 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7B9D34F-D145-4A75-9D49-07FB5008C9CA}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:AL32"/>
+  <dimension ref="A1:AN51"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="C11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="38" max="38" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="99.75">
+    <row r="1" spans="1:38" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -8824,7 +9722,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:38">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>13</v>
       </c>
@@ -8940,7 +9838,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="3" spans="1:38">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="109" t="s">
         <v>21</v>
       </c>
@@ -9054,7 +9952,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="4" spans="1:38">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="109" t="s">
         <v>21</v>
       </c>
@@ -9168,7 +10066,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="5" spans="1:38">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="72" t="s">
         <v>21</v>
       </c>
@@ -9282,7 +10180,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="6" spans="1:38">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="72" t="s">
         <v>21</v>
       </c>
@@ -9396,7 +10294,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="7" spans="1:38">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="72" t="s">
         <v>21</v>
       </c>
@@ -9510,7 +10408,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="8" spans="1:38">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" s="72" t="s">
         <v>21</v>
       </c>
@@ -9624,7 +10522,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="9" spans="1:38">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" s="72" t="s">
         <v>21</v>
       </c>
@@ -9738,7 +10636,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="10" spans="1:38">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="72" t="s">
         <v>21</v>
       </c>
@@ -9852,7 +10750,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="11" spans="1:38">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" s="72" t="s">
         <v>21</v>
       </c>
@@ -9966,7 +10864,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="12" spans="1:38">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" s="74" t="s">
         <v>21</v>
       </c>
@@ -10080,7 +10978,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="13" spans="1:38">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>21</v>
       </c>
@@ -10194,7 +11092,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="14" spans="1:38">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>21</v>
       </c>
@@ -10310,7 +11208,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="15" spans="1:38">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>21</v>
       </c>
@@ -10424,7 +11322,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="16" spans="1:38">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>21</v>
       </c>
@@ -10538,7 +11436,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="17" spans="1:38">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>21</v>
       </c>
@@ -10654,7 +11552,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="18" spans="1:38">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>21</v>
       </c>
@@ -10768,7 +11666,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="19" spans="1:38">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>21</v>
       </c>
@@ -10882,7 +11780,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="20" spans="1:38">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>21</v>
       </c>
@@ -10996,7 +11894,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="21" spans="1:38">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>21</v>
       </c>
@@ -11110,7 +12008,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="22" spans="1:38">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>21</v>
       </c>
@@ -11224,7 +12122,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="23" spans="1:38">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>21</v>
       </c>
@@ -11338,7 +12236,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="24" spans="1:38">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>21</v>
       </c>
@@ -11452,7 +12350,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="25" spans="1:38">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
         <v>21</v>
       </c>
@@ -11566,7 +12464,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="26" spans="1:38">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
         <v>21</v>
       </c>
@@ -11680,7 +12578,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="27" spans="1:38">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A27" s="119" t="s">
         <v>21</v>
       </c>
@@ -11794,7 +12692,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="28" spans="1:38">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A28" s="71" t="s">
         <v>21</v>
       </c>
@@ -11908,7 +12806,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="29" spans="1:38">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A29" s="71" t="s">
         <v>21</v>
       </c>
@@ -12022,7 +12920,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="30" spans="1:38">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A30" s="71" t="s">
         <v>21</v>
       </c>
@@ -12136,7 +13034,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="31" spans="1:38">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A31" s="72" t="s">
         <v>21</v>
       </c>
@@ -12250,7 +13148,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="32" spans="1:38">
+    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A32" s="134" t="s">
         <v>21</v>
       </c>
@@ -12362,6 +13260,557 @@
       </c>
       <c r="AL32" s="141" t="s">
         <v>869</v>
+      </c>
+    </row>
+    <row r="33" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="C33" s="9" t="s">
+        <v>989</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G33" s="162" t="s">
+        <v>990</v>
+      </c>
+      <c r="H33" s="163" t="s">
+        <v>993</v>
+      </c>
+      <c r="I33" s="163" t="s">
+        <v>996</v>
+      </c>
+      <c r="J33" s="164">
+        <v>2.6</v>
+      </c>
+      <c r="AN33" s="165">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="34" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="C34" s="13" t="s">
+        <v>989</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G34" s="166" t="s">
+        <v>991</v>
+      </c>
+      <c r="H34" s="167" t="s">
+        <v>994</v>
+      </c>
+      <c r="I34" s="167" t="s">
+        <v>997</v>
+      </c>
+      <c r="J34" s="168">
+        <v>3.6</v>
+      </c>
+      <c r="AN34" s="169">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="35" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="C35" s="15" t="s">
+        <v>989</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F35" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G35" s="93" t="s">
+        <v>992</v>
+      </c>
+      <c r="H35" s="94" t="s">
+        <v>995</v>
+      </c>
+      <c r="I35" s="94" t="s">
+        <v>998</v>
+      </c>
+      <c r="J35" s="95">
+        <v>3.6</v>
+      </c>
+      <c r="AN35" s="100">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="36" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="C36" s="15" t="s">
+        <v>989</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F36" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="G36" s="93">
+        <v>2.6</v>
+      </c>
+      <c r="H36" s="94">
+        <v>2.6</v>
+      </c>
+      <c r="I36" s="94">
+        <v>2.6</v>
+      </c>
+      <c r="J36" s="95">
+        <v>2.6</v>
+      </c>
+      <c r="AN36" s="100">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="37" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="C37" s="15" t="s">
+        <v>989</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F37" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G37" s="93">
+        <v>2.6</v>
+      </c>
+      <c r="H37" s="94">
+        <v>2.6</v>
+      </c>
+      <c r="I37" s="94">
+        <v>2.6</v>
+      </c>
+      <c r="J37" s="95">
+        <v>2.6</v>
+      </c>
+      <c r="AN37" s="100">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="38" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="C38" s="17" t="s">
+        <v>989</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F38" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G38" s="101">
+        <v>2.6</v>
+      </c>
+      <c r="H38" s="102">
+        <v>2.6</v>
+      </c>
+      <c r="I38" s="102">
+        <v>2.6</v>
+      </c>
+      <c r="J38" s="103">
+        <v>2.6</v>
+      </c>
+      <c r="AN38" s="108">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="39" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="C39" s="15" t="s">
+        <v>989</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F39" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="G39" s="93" t="s">
+        <v>999</v>
+      </c>
+      <c r="H39" s="94" t="s">
+        <v>1024</v>
+      </c>
+      <c r="I39" s="94" t="s">
+        <v>1025</v>
+      </c>
+      <c r="J39" s="95" t="s">
+        <v>1050</v>
+      </c>
+      <c r="AN39" s="100">
+        <v>45587</v>
+      </c>
+    </row>
+    <row r="40" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="C40" s="15" t="s">
+        <v>989</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F40" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G40" s="93" t="s">
+        <v>1000</v>
+      </c>
+      <c r="H40" s="94" t="s">
+        <v>1023</v>
+      </c>
+      <c r="I40" s="94" t="s">
+        <v>1026</v>
+      </c>
+      <c r="J40" s="95" t="s">
+        <v>1049</v>
+      </c>
+      <c r="AN40" s="100">
+        <v>45587</v>
+      </c>
+    </row>
+    <row r="41" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="C41" s="15" t="s">
+        <v>989</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E41" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F41" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="G41" s="93" t="s">
+        <v>1001</v>
+      </c>
+      <c r="H41" s="94" t="s">
+        <v>1022</v>
+      </c>
+      <c r="I41" s="94" t="s">
+        <v>1027</v>
+      </c>
+      <c r="J41" s="95" t="s">
+        <v>1048</v>
+      </c>
+      <c r="AN41" s="100">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="42" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="C42" s="15" t="s">
+        <v>989</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E42" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F42" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="G42" s="93" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H42" s="94" t="s">
+        <v>1021</v>
+      </c>
+      <c r="I42" s="94" t="s">
+        <v>1028</v>
+      </c>
+      <c r="J42" s="95" t="s">
+        <v>1047</v>
+      </c>
+      <c r="AN42" s="100">
+        <v>45587</v>
+      </c>
+    </row>
+    <row r="43" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="C43" s="15" t="s">
+        <v>989</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E43" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F43" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="G43" s="93" t="s">
+        <v>1003</v>
+      </c>
+      <c r="H43" s="94" t="s">
+        <v>1020</v>
+      </c>
+      <c r="I43" s="94" t="s">
+        <v>1029</v>
+      </c>
+      <c r="J43" s="95" t="s">
+        <v>1046</v>
+      </c>
+      <c r="AN43" s="100">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="44" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="C44" s="15" t="s">
+        <v>989</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E44" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F44" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="G44" s="93" t="s">
+        <v>1004</v>
+      </c>
+      <c r="H44" s="94" t="s">
+        <v>1019</v>
+      </c>
+      <c r="I44" s="94" t="s">
+        <v>1030</v>
+      </c>
+      <c r="J44" s="95" t="s">
+        <v>1045</v>
+      </c>
+      <c r="AN44" s="100">
+        <v>45587</v>
+      </c>
+    </row>
+    <row r="45" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="C45" s="15" t="s">
+        <v>989</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E45" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F45" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="G45" s="93" t="s">
+        <v>1005</v>
+      </c>
+      <c r="H45" s="94" t="s">
+        <v>1018</v>
+      </c>
+      <c r="I45" s="94" t="s">
+        <v>1031</v>
+      </c>
+      <c r="J45" s="95" t="s">
+        <v>1044</v>
+      </c>
+      <c r="AN45" s="100">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="46" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="C46" s="170" t="s">
+        <v>989</v>
+      </c>
+      <c r="D46" s="170" t="s">
+        <v>37</v>
+      </c>
+      <c r="E46" s="170" t="s">
+        <v>38</v>
+      </c>
+      <c r="F46" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="G46" s="171" t="s">
+        <v>1006</v>
+      </c>
+      <c r="H46" s="172" t="s">
+        <v>1017</v>
+      </c>
+      <c r="I46" s="172" t="s">
+        <v>1032</v>
+      </c>
+      <c r="J46" s="173" t="s">
+        <v>1043</v>
+      </c>
+      <c r="AN46" s="174">
+        <v>45587</v>
+      </c>
+    </row>
+    <row r="47" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="C47" s="15" t="s">
+        <v>989</v>
+      </c>
+      <c r="D47" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E47" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F47" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G47" s="93" t="s">
+        <v>1007</v>
+      </c>
+      <c r="H47" s="94" t="s">
+        <v>1016</v>
+      </c>
+      <c r="I47" s="94" t="s">
+        <v>1033</v>
+      </c>
+      <c r="J47" s="95" t="s">
+        <v>1042</v>
+      </c>
+      <c r="AN47" s="100">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="48" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="C48" s="15" t="s">
+        <v>989</v>
+      </c>
+      <c r="D48" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E48" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F48" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="G48" s="93" t="s">
+        <v>1008</v>
+      </c>
+      <c r="H48" s="94" t="s">
+        <v>1015</v>
+      </c>
+      <c r="I48" s="94" t="s">
+        <v>1034</v>
+      </c>
+      <c r="J48" s="95" t="s">
+        <v>1041</v>
+      </c>
+      <c r="AN48" s="100">
+        <v>45587</v>
+      </c>
+    </row>
+    <row r="49" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="C49" s="15" t="s">
+        <v>989</v>
+      </c>
+      <c r="D49" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E49" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F49" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="G49" s="93" t="s">
+        <v>1009</v>
+      </c>
+      <c r="H49" s="94" t="s">
+        <v>1014</v>
+      </c>
+      <c r="I49" s="94" t="s">
+        <v>1035</v>
+      </c>
+      <c r="J49" s="95" t="s">
+        <v>1040</v>
+      </c>
+      <c r="AN49" s="100">
+        <v>45587</v>
+      </c>
+    </row>
+    <row r="50" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="C50" s="170" t="s">
+        <v>989</v>
+      </c>
+      <c r="D50" s="170" t="s">
+        <v>37</v>
+      </c>
+      <c r="E50" s="170" t="s">
+        <v>42</v>
+      </c>
+      <c r="F50" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="G50" s="171" t="s">
+        <v>1010</v>
+      </c>
+      <c r="H50" s="172" t="s">
+        <v>1013</v>
+      </c>
+      <c r="I50" s="172" t="s">
+        <v>1036</v>
+      </c>
+      <c r="J50" s="173" t="s">
+        <v>1039</v>
+      </c>
+      <c r="AN50" s="174">
+        <v>45587</v>
+      </c>
+    </row>
+    <row r="51" spans="3:40" x14ac:dyDescent="0.25">
+      <c r="C51" s="17" t="s">
+        <v>989</v>
+      </c>
+      <c r="D51" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E51" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F51" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="G51" s="101" t="s">
+        <v>1011</v>
+      </c>
+      <c r="H51" s="102" t="s">
+        <v>1012</v>
+      </c>
+      <c r="I51" s="102" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J51" s="103" t="s">
+        <v>1038</v>
+      </c>
+      <c r="AN51" s="108">
+        <v>45587</v>
       </c>
     </row>
   </sheetData>
@@ -12380,7 +13829,7 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" style="7" bestFit="1" customWidth="1"/>
@@ -12405,7 +13854,7 @@
     <col min="31" max="16384" width="11.42578125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15" customHeight="1">
+    <row r="1" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12491,7 +13940,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>13</v>
       </c>
@@ -12581,7 +14030,7 @@
       </c>
       <c r="AD2" s="161"/>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>21</v>
       </c>
@@ -12672,7 +14121,7 @@
       </c>
       <c r="AD3" s="14"/>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>21</v>
       </c>
@@ -12762,7 +14211,7 @@
       </c>
       <c r="AD4" s="14"/>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>21</v>
       </c>
@@ -12852,7 +14301,7 @@
       </c>
       <c r="AD5" s="16"/>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>21</v>
       </c>
@@ -12942,7 +14391,7 @@
       </c>
       <c r="AD6" s="16"/>
     </row>
-    <row r="7" spans="1:30">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>21</v>
       </c>
@@ -13032,7 +14481,7 @@
       </c>
       <c r="AD7" s="16"/>
     </row>
-    <row r="8" spans="1:30">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>21</v>
       </c>
@@ -13122,7 +14571,7 @@
       </c>
       <c r="AD8" s="16"/>
     </row>
-    <row r="9" spans="1:30">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>21</v>
       </c>
@@ -13212,7 +14661,7 @@
       </c>
       <c r="AD9" s="16"/>
     </row>
-    <row r="10" spans="1:30">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>21</v>
       </c>
@@ -13302,7 +14751,7 @@
       </c>
       <c r="AD10" s="16"/>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>21</v>
       </c>
@@ -13392,7 +14841,7 @@
       </c>
       <c r="AD11" s="16"/>
     </row>
-    <row r="12" spans="1:30">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>21</v>
       </c>
@@ -13482,7 +14931,7 @@
       </c>
       <c r="AD12" s="18"/>
     </row>
-    <row r="13" spans="1:30">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>21</v>
       </c>
@@ -13572,7 +15021,7 @@
       </c>
       <c r="AD13" s="16"/>
     </row>
-    <row r="14" spans="1:30">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>21</v>
       </c>
@@ -13662,7 +15111,7 @@
       </c>
       <c r="AD14" s="16"/>
     </row>
-    <row r="15" spans="1:30">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>21</v>
       </c>
@@ -13752,7 +15201,7 @@
       </c>
       <c r="AD15" s="16"/>
     </row>
-    <row r="16" spans="1:30">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>21</v>
       </c>
@@ -13842,7 +15291,7 @@
       </c>
       <c r="AD16" s="16"/>
     </row>
-    <row r="17" spans="1:30">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>21</v>
       </c>
@@ -13932,7 +15381,7 @@
       </c>
       <c r="AD17" s="16"/>
     </row>
-    <row r="18" spans="1:30">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>21</v>
       </c>
@@ -14022,7 +15471,7 @@
       </c>
       <c r="AD18" s="16"/>
     </row>
-    <row r="19" spans="1:30">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>21</v>
       </c>
@@ -14112,7 +15561,7 @@
       </c>
       <c r="AD19" s="16"/>
     </row>
-    <row r="20" spans="1:30">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>21</v>
       </c>
@@ -14202,7 +15651,7 @@
       </c>
       <c r="AD20" s="16"/>
     </row>
-    <row r="21" spans="1:30">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>21</v>
       </c>
@@ -14292,7 +15741,7 @@
       </c>
       <c r="AD21" s="16"/>
     </row>
-    <row r="22" spans="1:30">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>21</v>
       </c>
@@ -14382,7 +15831,7 @@
       </c>
       <c r="AD22" s="16"/>
     </row>
-    <row r="23" spans="1:30">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>21</v>
       </c>
@@ -14472,7 +15921,7 @@
       </c>
       <c r="AD23" s="16"/>
     </row>
-    <row r="24" spans="1:30">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>21</v>
       </c>
@@ -14562,7 +16011,7 @@
       </c>
       <c r="AD24" s="16"/>
     </row>
-    <row r="25" spans="1:30">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
         <v>21</v>
       </c>
@@ -14652,7 +16101,7 @@
       </c>
       <c r="AD25" s="16"/>
     </row>
-    <row r="26" spans="1:30">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>21</v>
       </c>
@@ -14742,7 +16191,7 @@
       </c>
       <c r="AD26" s="10"/>
     </row>
-    <row r="27" spans="1:30">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>21</v>
       </c>
@@ -14832,7 +16281,7 @@
       </c>
       <c r="AD27" s="16"/>
     </row>
-    <row r="28" spans="1:30">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
         <v>21</v>
       </c>
@@ -14922,7 +16371,7 @@
       </c>
       <c r="AD28" s="16"/>
     </row>
-    <row r="29" spans="1:30">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
         <v>21</v>
       </c>
@@ -15012,7 +16461,7 @@
       </c>
       <c r="AD29" s="16"/>
     </row>
-    <row r="30" spans="1:30">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
         <v>21</v>
       </c>
@@ -15102,7 +16551,7 @@
       </c>
       <c r="AD30" s="16"/>
     </row>
-    <row r="31" spans="1:30">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
         <v>21</v>
       </c>
@@ -15192,7 +16641,7 @@
       </c>
       <c r="AD31" s="16"/>
     </row>
-    <row r="32" spans="1:30">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>21</v>
       </c>
@@ -15282,22 +16731,22 @@
       </c>
       <c r="AD32" s="18"/>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
     </row>
   </sheetData>
@@ -15318,23 +16767,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="c5381946-f1d1-449f-b695-d98d204cc1c9">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="c5381946-f1d1-449f-b695-d98d204cc1c9" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="75c5e37f-bc1e-40b7-ac00-1ab7acfb489c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -15604,22 +17042,29 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="c5381946-f1d1-449f-b695-d98d204cc1c9">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="c5381946-f1d1-449f-b695-d98d204cc1c9" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="75c5e37f-bc1e-40b7-ac00-1ab7acfb489c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{990DCB4B-FBBF-4997-8C1B-1027DBEC0554}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47809CAB-73CD-4E13-B718-ADA289F0A22D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c5381946-f1d1-449f-b695-d98d204cc1c9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="75c5e37f-bc1e-40b7-ac00-1ab7acfb489c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -15645,9 +17090,13 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47809CAB-73CD-4E13-B718-ADA289F0A22D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{990DCB4B-FBBF-4997-8C1B-1027DBEC0554}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c5381946-f1d1-449f-b695-d98d204cc1c9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="75c5e37f-bc1e-40b7-ac00-1ab7acfb489c"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>